<commit_message>
Changed X1 quartz value.
</commit_message>
<xml_diff>
--- a/PCB/PCB_project_v4/TOF_rangefinder_v4b.xlsx
+++ b/PCB/PCB_project_v4/TOF_rangefinder_v4b.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="166">
   <si>
     <t>Designator</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>8 MHz</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
   </si>
 </sst>
 </file>
@@ -911,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2159,7 +2162,7 @@
         <v>160</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>35</v>

</xml_diff>